<commit_message>
Actualización mapa conceptual tema 3 math 8
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
@@ -6338,8 +6338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:E35"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6358,7 +6358,7 @@
     <col min="12" max="12" width="15.5703125" style="60" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" style="60" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" style="60" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" style="60" customWidth="1"/>
+    <col min="15" max="15" width="58" style="60" customWidth="1"/>
     <col min="16" max="16" width="15.28515625" style="60" customWidth="1"/>
     <col min="17" max="17" width="10.140625" style="86" customWidth="1"/>
     <col min="18" max="18" width="14" style="86" customWidth="1"/>

</xml_diff>

<commit_message>
Asignación de recursos Autoria Clara
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion03\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7755"/>
   </bookViews>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="267">
   <si>
     <t>Asignatura</t>
   </si>
@@ -880,6 +885,9 @@
   </si>
   <si>
     <t>Recurso M101A-04</t>
+  </si>
+  <si>
+    <t>Clara</t>
   </si>
 </sst>
 </file>
@@ -1340,6 +1348,15 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1371,15 +1388,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1442,7 +1450,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1477,7 +1485,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1688,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BG131" sqref="BG130:BH131"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19:V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,95 +1728,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="95" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="94" t="s">
         <v>237</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="99" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="99" t="s">
         <v>239</v>
       </c>
-      <c r="I1" s="96" t="s">
+      <c r="I1" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="94" t="s">
+      <c r="J1" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="L1" s="93" t="s">
+      <c r="L1" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="98" t="s">
+      <c r="M1" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="98"/>
-      <c r="O1" s="99" t="s">
+      <c r="N1" s="101"/>
+      <c r="O1" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="90" t="s">
+      <c r="P1" s="93" t="s">
         <v>242</v>
       </c>
-      <c r="Q1" s="100" t="s">
+      <c r="Q1" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="102" t="s">
+      <c r="R1" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="100" t="s">
+      <c r="S1" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="101" t="s">
+      <c r="T1" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="100" t="s">
+      <c r="U1" s="89" t="s">
         <v>91</v>
       </c>
       <c r="V1" s="59"/>
     </row>
     <row r="2" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="93"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="96"/>
       <c r="M2" s="61" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="99"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="100"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="89"/>
       <c r="V2" s="59"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1931,7 +1939,9 @@
       <c r="U4" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V4" s="59"/>
+      <c r="V4" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
@@ -1991,7 +2001,9 @@
       <c r="U5" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V5" s="59"/>
+      <c r="V5" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
@@ -2051,7 +2063,9 @@
       <c r="U6" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V6" s="59"/>
+      <c r="V6" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
@@ -2113,7 +2127,9 @@
       <c r="U7" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V7" s="59"/>
+      <c r="V7" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
@@ -2175,7 +2191,9 @@
       <c r="U8" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V8" s="59"/>
+      <c r="V8" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
@@ -2357,7 +2375,9 @@
       <c r="U11" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V11" s="59"/>
+      <c r="V11" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
@@ -2417,7 +2437,9 @@
       <c r="U12" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V12" s="59"/>
+      <c r="V12" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
@@ -2479,7 +2501,9 @@
       <c r="U13" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V13" s="59"/>
+      <c r="V13" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
@@ -2541,7 +2565,9 @@
       <c r="U14" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V14" s="59"/>
+      <c r="V14" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
@@ -2603,7 +2629,9 @@
       <c r="U15" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V15" s="59"/>
+      <c r="V15" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
@@ -2665,7 +2693,9 @@
       <c r="U16" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V16" s="59"/>
+      <c r="V16" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
@@ -2849,7 +2879,9 @@
       <c r="U19" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V19" s="59"/>
+      <c r="V19" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
@@ -2913,7 +2945,9 @@
       <c r="U20" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V20" s="59"/>
+      <c r="V20" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
@@ -2977,7 +3011,9 @@
       <c r="U21" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V21" s="59"/>
+      <c r="V21" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
@@ -3039,7 +3075,9 @@
       <c r="U22" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V22" s="59"/>
+      <c r="V22" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
@@ -3101,7 +3139,9 @@
       <c r="U23" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V23" s="59"/>
+      <c r="V23" s="59" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="49" t="s">
@@ -4031,30 +4071,30 @@
       <c r="U43" s="82"/>
     </row>
     <row r="44" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="89"/>
-      <c r="B44" s="89"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
-      <c r="G44" s="89"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="89"/>
-      <c r="J44" s="89"/>
-      <c r="K44" s="89"/>
+      <c r="A44" s="92"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="92"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="92"/>
+      <c r="K44" s="92"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="89"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="89"/>
-      <c r="G45" s="89"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
+      <c r="A45" s="92"/>
+      <c r="B45" s="92"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="92"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="P46" s="60" t="s">
@@ -4087,11 +4127,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
     <mergeCell ref="A44:K45"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="B1:B2"/>
@@ -4108,6 +4143,11 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L78 K3:K43">
@@ -4128,7 +4168,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M78 L3:L43">
       <formula1>$C$50:$K$50</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V18 P3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3">
       <formula1>$W$20:$W$20</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Asignación recursos mat 9 tema 3
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="273">
   <si>
     <t>Asignatura</t>
   </si>
@@ -888,6 +888,24 @@
   </si>
   <si>
     <t>Clara</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Andrea Sabogal</t>
+  </si>
+  <si>
+    <t>Cristhian Bello</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Joahnna Vera</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1005,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1069,6 +1087,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1154,7 +1184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1348,15 +1378,6 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1390,6 +1411,17 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1696,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19:V23"/>
+    <sheetView tabSelected="1" topLeftCell="K13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1728,95 +1760,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="92" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="91" t="s">
         <v>237</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="99" t="s">
+      <c r="H1" s="96" t="s">
         <v>239</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="96" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="97" t="s">
+      <c r="J1" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="100" t="s">
+      <c r="K1" s="97" t="s">
         <v>241</v>
       </c>
-      <c r="L1" s="96" t="s">
+      <c r="L1" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="101" t="s">
+      <c r="M1" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="101"/>
-      <c r="O1" s="102" t="s">
+      <c r="N1" s="98"/>
+      <c r="O1" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="93" t="s">
+      <c r="P1" s="90" t="s">
         <v>242</v>
       </c>
-      <c r="Q1" s="89" t="s">
+      <c r="Q1" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="91" t="s">
+      <c r="R1" s="102" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="89" t="s">
+      <c r="S1" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="90" t="s">
+      <c r="T1" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="89" t="s">
+      <c r="U1" s="100" t="s">
         <v>91</v>
       </c>
       <c r="V1" s="59"/>
     </row>
     <row r="2" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="96"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="93"/>
       <c r="M2" s="61" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="102"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="89"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="100"/>
       <c r="V2" s="59"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1877,7 +1909,9 @@
       <c r="U3" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="V3" s="59"/>
+      <c r="V3" s="63" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
@@ -2255,7 +2289,9 @@
       <c r="U9" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V9" s="59"/>
+      <c r="V9" s="63" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
@@ -2315,7 +2351,9 @@
       <c r="U10" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="V10" s="59"/>
+      <c r="V10" s="103" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
@@ -2757,7 +2795,9 @@
       <c r="U17" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V17" s="59"/>
+      <c r="V17" s="103" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
@@ -2817,7 +2857,9 @@
       <c r="U18" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="V18" s="59"/>
+      <c r="V18" s="104" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
@@ -3205,7 +3247,9 @@
       <c r="U24" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="V24" s="59"/>
+      <c r="V24" s="104" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="49" t="s">
@@ -3269,7 +3313,9 @@
       <c r="U25" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V25" s="59"/>
+      <c r="V25" s="63" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
@@ -3331,7 +3377,9 @@
       <c r="U26" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V26" s="59"/>
+      <c r="V26" s="104" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
@@ -3393,7 +3441,9 @@
       <c r="U27" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V27" s="59"/>
+      <c r="V27" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
@@ -3455,7 +3505,9 @@
       <c r="U28" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="V28" s="59"/>
+      <c r="V28" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
@@ -3517,7 +3569,9 @@
       <c r="U29" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V29" s="59"/>
+      <c r="V29" s="104" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
@@ -3579,7 +3633,9 @@
       <c r="U30" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V30" s="59"/>
+      <c r="V30" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
@@ -3639,7 +3695,9 @@
       <c r="U31" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="V31" s="59"/>
+      <c r="V31" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="49" t="s">
@@ -3699,7 +3757,9 @@
       <c r="U32" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V32" s="59"/>
+      <c r="V32" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
@@ -3759,7 +3819,9 @@
       <c r="U33" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V33" s="59"/>
+      <c r="V33" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
@@ -3801,7 +3863,9 @@
       <c r="S34" s="79"/>
       <c r="T34" s="81"/>
       <c r="U34" s="79"/>
-      <c r="V34" s="59"/>
+      <c r="V34" s="59" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="49" t="s">
@@ -3859,7 +3923,9 @@
       <c r="U35" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V35" s="59"/>
+      <c r="V35" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="49" t="s">
@@ -3907,7 +3973,9 @@
       <c r="U36" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="V36" s="59"/>
+      <c r="V36" s="59" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="37" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="42"/>
@@ -4071,30 +4139,30 @@
       <c r="U43" s="82"/>
     </row>
     <row r="44" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="92"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="92"/>
-      <c r="H44" s="92"/>
-      <c r="I44" s="92"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="92"/>
+      <c r="A44" s="89"/>
+      <c r="B44" s="89"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="89"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="89"/>
+      <c r="J44" s="89"/>
+      <c r="K44" s="89"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="92"/>
-      <c r="B45" s="92"/>
-      <c r="C45" s="92"/>
-      <c r="D45" s="92"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="92"/>
-      <c r="I45" s="92"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="92"/>
+      <c r="A45" s="89"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="P46" s="60" t="s">
@@ -4127,6 +4195,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
     <mergeCell ref="A44:K45"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="B1:B2"/>
@@ -4143,11 +4216,6 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:O2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L78 K3:K43">

</xml_diff>

<commit_message>
RevisionPlataforma_MA_09_03_CO_1, ESCALETA_MA_09_03_CO y Formulas_MA_09_03_CO
RevisionPlataforma_MA_09_03_CO_1, ESCALETA_MA_09_03_CO actualizada y
carpeta de Formulas_MA_09_03_CO actualizada
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion03/ESCALETA_MA_09_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS PLANETA. FERNANDA\ESCALETAS\ESCALETA_MA_09_03_CO\ESCALETAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="275">
   <si>
     <t>Asignatura</t>
   </si>
@@ -339,12 +339,6 @@
     <t>La necesidad de ampliar el conjunto de los números reales</t>
   </si>
   <si>
-    <t>Interactivo que expone la necesidad de ampliar los conjuntos numéricos</t>
-  </si>
-  <si>
-    <t>Actividad que permite identificar números que pertenecen a cada conjunto numérico</t>
-  </si>
-  <si>
     <t>Los números imaginarios</t>
   </si>
   <si>
@@ -366,18 +360,12 @@
     <t>Practica el cálculo del módulo de un número complejo</t>
   </si>
   <si>
-    <t>Actividad que permite identificar el módulo de un número complejo</t>
-  </si>
-  <si>
     <t>Original REC60</t>
   </si>
   <si>
     <t>Identifica el conjugado de un número complejo</t>
   </si>
   <si>
-    <t>Actividad que permite identificar el conjugado de un número complejo</t>
-  </si>
-  <si>
     <t>Consolidación</t>
   </si>
   <si>
@@ -396,15 +384,9 @@
     <t>La adición de números complejos</t>
   </si>
   <si>
-    <t xml:space="preserve">Interactivo que expone la adición de números complejos </t>
-  </si>
-  <si>
     <t>Practica la adición de números complejos</t>
   </si>
   <si>
-    <t>Actividad que permite la ejercitación de la adición de números complejos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Original REC90 Revisar redacción de las preguntas. </t>
   </si>
   <si>
@@ -414,12 +396,6 @@
     <t>Practica las propiedades de la adición de números complejos</t>
   </si>
   <si>
-    <t>Identifica las propiedades de la adición de los números complejos</t>
-  </si>
-  <si>
-    <t>Actividad para identificar las propiedades de la adición a partir de un ejemplo</t>
-  </si>
-  <si>
     <t>Original REC100</t>
   </si>
   <si>
@@ -438,24 +414,12 @@
     <t>Las propiedades de la multiplicación de números complejos</t>
   </si>
   <si>
-    <t xml:space="preserve">Propiedades de la multiplicación de números complejos </t>
-  </si>
-  <si>
     <t>Practica la multiplicación de números complejos</t>
   </si>
   <si>
-    <t>Actividad que permite la ejercitación de la multiplicación de números complejos</t>
-  </si>
-  <si>
-    <t>Interactivo que expone las propiedades de la multiplicación de números complejos</t>
-  </si>
-  <si>
     <t>Identifica las propiedades de la multiplicación de números complejos</t>
   </si>
   <si>
-    <t>Actividad que permite identificar las propiedades de la multiplicación de números complejos a partir de ejemplos</t>
-  </si>
-  <si>
     <t>Original REC140</t>
   </si>
   <si>
@@ -474,21 +438,12 @@
     <t>Se explican todas las propiedades de la multiplicación de números complejos. Tener en cuenta que se debe incluir el inverso multiplicativo (puede ser cuando se habla del elemeto neutro)</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: identifica el conjunto numérico al que pertenece la solución de cada operación </t>
-  </si>
-  <si>
-    <t>Actividad para identificar el conjunto numérico al cual pertenece la solución de las operaciones propuestas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Original REC10. Incluir operaciones diferentes a la adición y que se utilicen las propiedades. </t>
   </si>
   <si>
     <t>Aplicaciones de los números complejos</t>
   </si>
   <si>
-    <t>Interactivo que expone brevemente algunas aplicaciones de los números complejos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Diaporama: exponer gráficamente algunas aplicaciones de los números complejos, por ejemplo: electrónica, fractales, mecánica, cuántica, etc. </t>
   </si>
   <si>
@@ -498,9 +453,6 @@
     <t>Proyecto: los fractales</t>
   </si>
   <si>
-    <t>Proyecto que permite analizar los números complejos aplicados en los fractales</t>
-  </si>
-  <si>
     <t>Proponer un proyecto que permita realizar una investigación de los números complejos aplicados en los fractales y que de como resultado la exposición o puesta en escenta de varias imágenes de fractales o creación de los mismos en material concreto (p.e. papel)</t>
   </si>
   <si>
@@ -513,9 +465,6 @@
     <t>Original REC180</t>
   </si>
   <si>
-    <t>Actividad que propone ejercicios para validar las habilidades desarrolladas con los números complejos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Redactar el recurso con lo expuesto originalmente en el guión. La idea es que se muestre las diferentes ampliaciones de los conjuntos numéricos, en lo posible, a partir de situaciones problema y a medida que se va haciendo la explicación, hacer pregntas a los estudiantes que los lleve a evidenciar dicha necesidad. </t>
   </si>
   <si>
@@ -618,9 +567,6 @@
     <t>Actividad para identificar números imaginarios puros</t>
   </si>
   <si>
-    <t>Reconoce números imagianrios puros</t>
-  </si>
-  <si>
     <t>Dos contenedores. Uno con número imaginarios puro y el otro con  números reales. El estudiante debe clasificar las cantidades que se indiquen en las distintas filas.</t>
   </si>
   <si>
@@ -639,27 +585,15 @@
     <t>En la figura de la izquierda deben proponerse varias ecuaciones de segundo grado cuyas soluciones sean raíces negativas. Enlas alternativas de la derecha, colocar resultados en los cuales se involucren varias alternativas similares, por ejemplo raíz negativa; raíz con radicando negativa, raíz positiva, solo el radicando, etc. tener en cuenta que las ecuaciuones pueden tener dos soluciones.</t>
   </si>
   <si>
-    <t>Resuelve ecuaciones</t>
-  </si>
-  <si>
-    <t>Actividad para resovolver ecuaciones que involucran números imaginarios</t>
-  </si>
-  <si>
     <t>Los números complejos</t>
   </si>
   <si>
     <t xml:space="preserve">Mostrar en el recurso un breve historia del conjunto de los números complejos, su definición, su escritura como pareja de coordenadas cartesianas, su representación en el plano. </t>
   </si>
   <si>
-    <t>Interactivo que explica el conjunto de los números complejos</t>
-  </si>
-  <si>
     <t>Identifica números complejos en el plano cartesiano</t>
   </si>
   <si>
-    <t>Actividad para escribir en forma binomial el número complejo representado en el plano</t>
-  </si>
-  <si>
     <t>Dar cuatro o más planos cartesianos cuyos ejes son el eje imaginario y el eje real. Nombrar cada punto con una letra mayúscula. El estudiante debe escribir el número representado en la forma compleja. Tener en cuenta que solo se escriban números enteros.</t>
   </si>
   <si>
@@ -687,9 +621,6 @@
     <t>Debe darse la explicación de las operaciones con números complejos. Adición, sustracción, multiplicación y división. Incluyendo propiedades e inverso multiplicativo. Mostrar ejemplos.</t>
   </si>
   <si>
-    <t>Actividad para ejercitar la adición y la sustracción de  números complejos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Proponer operaciones de adición y de sustracción. Incluir aquellas que contienen signos de agrupación. </t>
   </si>
   <si>
@@ -708,25 +639,13 @@
     <t>Preguntas abiertas sobre los temas trabajados con las operaciones entre números reales.</t>
   </si>
   <si>
-    <t>Actividad sobre Las aplicaciones de los números complejos</t>
-  </si>
-  <si>
     <t>Determina la norma de un número complejo</t>
   </si>
   <si>
-    <t>Actividades para calcular la norma de un número complejo</t>
-  </si>
-  <si>
     <t>Los estudiantes deben calcular la norma de un número complejo</t>
   </si>
   <si>
-    <t>Competencias: profundiza acerca de las aplicaciones de los números complejos</t>
-  </si>
-  <si>
     <t>Proponer la profundización o investigación de las aplicaciones descritas en el REC361</t>
-  </si>
-  <si>
-    <t>Mapa conceptual sobre el tema Los números complejos</t>
   </si>
   <si>
     <t>Evaluación</t>
@@ -906,6 +825,93 @@
   </si>
   <si>
     <t>Joahnna Vera</t>
+  </si>
+  <si>
+    <t>Interactivo para explicar la necesidad de ampliar los conjuntos numéricos</t>
+  </si>
+  <si>
+    <t>Actividad que permite clasificar números que pertenecen a un conjunto numérico</t>
+  </si>
+  <si>
+    <t>Reconoce números imaginarios puros</t>
+  </si>
+  <si>
+    <t>Resuelve ecuaciones con números imaginarios</t>
+  </si>
+  <si>
+    <t>Actividad para resolver ecuaciones que involucran números imaginarios</t>
+  </si>
+  <si>
+    <t>Interactivo para explicar el conjunto de los números complejos</t>
+  </si>
+  <si>
+    <t>Actividad para escribir en forma binomial un número complejo representado en el plano</t>
+  </si>
+  <si>
+    <t>Actividad para identificar el módulo de un número complejo</t>
+  </si>
+  <si>
+    <t>Actividad para identificar el conjugado de un número complejo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo para explicar las operaciones con números complejos </t>
+  </si>
+  <si>
+    <t>Actividad para ejercitar la adición de números complejos</t>
+  </si>
+  <si>
+    <t>Actividad para practicar las propiedades de la adición de números complejos</t>
+  </si>
+  <si>
+    <t>Actividad para identificar las propiedades de la adición de números complejos</t>
+  </si>
+  <si>
+    <t>Actividad para practicar la multiplicación de números complejos</t>
+  </si>
+  <si>
+    <t>Interactivo para exponer las propiedades de la multiplicación de números complejos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para identificar las propiedades de la multiplicación de números complejos </t>
+  </si>
+  <si>
+    <t>Actividad para calcular la norma de un número complejo</t>
+  </si>
+  <si>
+    <t>Interactivo que muestra algunas aplicaciones de los números complejos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifica el conjunto numérico al que pertenece el resultado de una operación </t>
+  </si>
+  <si>
+    <t>Actividad para identificar el conjunto numérico al cual pertenece el resultado de una operación</t>
+  </si>
+  <si>
+    <t>Proyecto sobre los números complejos y los fractales</t>
+  </si>
+  <si>
+    <t>Competencias: los circuitos eléctricos y los números complejos</t>
+  </si>
+  <si>
+    <t>Actividad sobre los circuitos eléctrios y los números complejos</t>
+  </si>
+  <si>
+    <t>Banco de actividades: Los números complejos</t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema Los números complejos</t>
+  </si>
+  <si>
+    <t>Actividad para evaluar el tema Los números complejos</t>
+  </si>
+  <si>
+    <t>Actividad de respuesta abierta sobre Los números complejos</t>
+  </si>
+  <si>
+    <t>Identifica las propiedades de la adición de números complejos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las propiedades de la multiplicación de números complejos </t>
   </si>
 </sst>
 </file>
@@ -1378,6 +1384,8 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1420,8 +1428,6 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1728,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView tabSelected="1" topLeftCell="K19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,95 +1766,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="92" t="s">
-        <v>236</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>237</v>
-      </c>
-      <c r="F1" s="96" t="s">
-        <v>238</v>
-      </c>
-      <c r="G1" s="93" t="s">
+      <c r="D1" s="94" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="93" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="98" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="96" t="s">
-        <v>239</v>
-      </c>
-      <c r="I1" s="96" t="s">
-        <v>240</v>
-      </c>
-      <c r="J1" s="94" t="s">
+      <c r="H1" s="98" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="98" t="s">
+        <v>213</v>
+      </c>
+      <c r="J1" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="97" t="s">
-        <v>241</v>
-      </c>
-      <c r="L1" s="93" t="s">
+      <c r="K1" s="99" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="98" t="s">
+      <c r="M1" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="98"/>
-      <c r="O1" s="99" t="s">
+      <c r="N1" s="100"/>
+      <c r="O1" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="90" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q1" s="100" t="s">
+      <c r="P1" s="92" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q1" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="102" t="s">
+      <c r="R1" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="100" t="s">
+      <c r="S1" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="101" t="s">
+      <c r="T1" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="100" t="s">
+      <c r="U1" s="102" t="s">
         <v>91</v>
       </c>
       <c r="V1" s="59"/>
     </row>
     <row r="2" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="93"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="95"/>
       <c r="M2" s="61" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="99"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="100"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="102"/>
       <c r="V2" s="59"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1859,7 +1865,7 @@
         <v>102</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D3" s="52" t="s">
         <v>104</v>
@@ -1876,7 +1882,7 @@
         <v>100</v>
       </c>
       <c r="J3" s="62" t="s">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="K3" s="55" t="s">
         <v>101</v>
@@ -1889,7 +1895,7 @@
       </c>
       <c r="N3" s="57"/>
       <c r="O3" s="74" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="P3" s="76" t="s">
         <v>100</v>
@@ -1898,19 +1904,19 @@
         <v>6</v>
       </c>
       <c r="R3" s="80" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="S3" s="79" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="T3" s="81" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="U3" s="79" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="V3" s="63" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -1921,17 +1927,17 @@
         <v>102</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D4" s="52" t="s">
         <v>104</v>
       </c>
       <c r="E4" s="63" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F4" s="74"/>
       <c r="G4" s="58" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="H4" s="76">
         <v>2</v>
@@ -1940,7 +1946,7 @@
         <v>101</v>
       </c>
       <c r="J4" s="62" t="s">
-        <v>106</v>
+        <v>247</v>
       </c>
       <c r="K4" s="55" t="s">
         <v>101</v>
@@ -1953,7 +1959,7 @@
         <v>98</v>
       </c>
       <c r="O4" s="74" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="P4" s="76" t="s">
         <v>100</v>
@@ -1962,19 +1968,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S4" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T4" s="81" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="U4" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V4" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1985,7 +1991,7 @@
         <v>102</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D5" s="52" t="s">
         <v>104</v>
@@ -1993,7 +1999,7 @@
       <c r="E5" s="63"/>
       <c r="F5" s="74"/>
       <c r="G5" s="58" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="H5" s="76">
         <v>3</v>
@@ -2002,7 +2008,7 @@
         <v>101</v>
       </c>
       <c r="J5" s="62" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="K5" s="55" t="s">
         <v>101</v>
@@ -2015,7 +2021,7 @@
         <v>83</v>
       </c>
       <c r="O5" s="74" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="P5" s="76" t="s">
         <v>100</v>
@@ -2024,19 +2030,19 @@
         <v>6</v>
       </c>
       <c r="R5" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S5" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T5" s="81" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="U5" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V5" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -2047,7 +2053,7 @@
         <v>102</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D6" s="52" t="s">
         <v>104</v>
@@ -2055,7 +2061,7 @@
       <c r="E6" s="63"/>
       <c r="F6" s="74"/>
       <c r="G6" s="58" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="H6" s="76">
         <v>4</v>
@@ -2064,7 +2070,7 @@
         <v>101</v>
       </c>
       <c r="J6" s="62" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="K6" s="55" t="s">
         <v>101</v>
@@ -2077,7 +2083,7 @@
         <v>96</v>
       </c>
       <c r="O6" s="74" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="P6" s="76" t="s">
         <v>100</v>
@@ -2086,19 +2092,19 @@
         <v>6</v>
       </c>
       <c r="R6" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S6" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T6" s="81" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="U6" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V6" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -2109,17 +2115,17 @@
         <v>102</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D7" s="52" t="s">
         <v>104</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="F7" s="74"/>
       <c r="G7" s="58" t="s">
-        <v>205</v>
+        <v>249</v>
       </c>
       <c r="H7" s="76">
         <v>5</v>
@@ -2128,7 +2134,7 @@
         <v>101</v>
       </c>
       <c r="J7" s="62" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="K7" s="55" t="s">
         <v>101</v>
@@ -2141,7 +2147,7 @@
         <v>82</v>
       </c>
       <c r="O7" s="74" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="P7" s="76" t="s">
         <v>101</v>
@@ -2150,19 +2156,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S7" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T7" s="81" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="U7" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V7" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2173,17 +2179,17 @@
         <v>102</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D8" s="52" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F8" s="74"/>
       <c r="G8" s="58" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="H8" s="76">
         <v>6</v>
@@ -2192,7 +2198,7 @@
         <v>101</v>
       </c>
       <c r="J8" s="62" t="s">
-        <v>255</v>
+        <v>228</v>
       </c>
       <c r="K8" s="55" t="s">
         <v>101</v>
@@ -2205,7 +2211,7 @@
         <v>95</v>
       </c>
       <c r="O8" s="74" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="P8" s="76" t="s">
         <v>100</v>
@@ -2214,19 +2220,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S8" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T8" s="81" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="U8" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V8" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2237,17 +2243,17 @@
         <v>102</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>104</v>
       </c>
       <c r="E9" s="63" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F9" s="74"/>
       <c r="G9" s="58" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="H9" s="76">
         <v>7</v>
@@ -2256,7 +2262,7 @@
         <v>101</v>
       </c>
       <c r="J9" s="62" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="K9" s="55" t="s">
         <v>101</v>
@@ -2269,7 +2275,7 @@
         <v>84</v>
       </c>
       <c r="O9" s="74" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
       <c r="P9" s="76" t="s">
         <v>100</v>
@@ -2278,19 +2284,19 @@
         <v>6</v>
       </c>
       <c r="R9" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S9" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T9" s="81" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="U9" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V9" s="63" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2301,15 +2307,15 @@
         <v>102</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E10" s="63"/>
       <c r="F10" s="74"/>
       <c r="G10" s="58" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="H10" s="76">
         <v>8</v>
@@ -2318,7 +2324,7 @@
         <v>100</v>
       </c>
       <c r="J10" s="62" t="s">
-        <v>209</v>
+        <v>251</v>
       </c>
       <c r="K10" s="55" t="s">
         <v>101</v>
@@ -2331,7 +2337,7 @@
       </c>
       <c r="N10" s="57"/>
       <c r="O10" s="74" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="P10" s="76" t="s">
         <v>100</v>
@@ -2340,19 +2346,19 @@
         <v>6</v>
       </c>
       <c r="R10" s="80" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="S10" s="79" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="T10" s="81" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="U10" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="V10" s="103" t="s">
-        <v>268</v>
+        <v>151</v>
+      </c>
+      <c r="V10" s="89" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2363,15 +2369,15 @@
         <v>102</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E11" s="63"/>
       <c r="F11" s="74"/>
       <c r="G11" s="58" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="H11" s="76">
         <v>9</v>
@@ -2380,7 +2386,7 @@
         <v>101</v>
       </c>
       <c r="J11" s="62" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="K11" s="55" t="s">
         <v>101</v>
@@ -2393,7 +2399,7 @@
         <v>81</v>
       </c>
       <c r="O11" s="74" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="P11" s="76" t="s">
         <v>100</v>
@@ -2402,19 +2408,19 @@
         <v>6</v>
       </c>
       <c r="R11" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S11" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T11" s="81" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="U11" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V11" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2425,15 +2431,15 @@
         <v>102</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E12" s="63"/>
       <c r="F12" s="74"/>
       <c r="G12" s="58" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="H12" s="76">
         <v>10</v>
@@ -2442,7 +2448,7 @@
         <v>101</v>
       </c>
       <c r="J12" s="62" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="K12" s="55" t="s">
         <v>101</v>
@@ -2455,7 +2461,7 @@
         <v>98</v>
       </c>
       <c r="O12" s="74" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="P12" s="76" t="s">
         <v>100</v>
@@ -2464,19 +2470,19 @@
         <v>6</v>
       </c>
       <c r="R12" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S12" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T12" s="81" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="U12" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V12" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -2487,17 +2493,17 @@
         <v>102</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D13" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F13" s="74"/>
       <c r="G13" s="58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H13" s="76">
         <v>11</v>
@@ -2506,7 +2512,7 @@
         <v>101</v>
       </c>
       <c r="J13" s="62" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K13" s="55" t="s">
         <v>101</v>
@@ -2519,7 +2525,7 @@
         <v>94</v>
       </c>
       <c r="O13" s="74" t="s">
-        <v>260</v>
+        <v>233</v>
       </c>
       <c r="P13" s="76" t="s">
         <v>100</v>
@@ -2528,19 +2534,19 @@
         <v>6</v>
       </c>
       <c r="R13" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S13" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T13" s="81" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="U13" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V13" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2551,17 +2557,17 @@
         <v>102</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D14" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F14" s="74"/>
       <c r="G14" s="58" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H14" s="76">
         <v>12</v>
@@ -2570,7 +2576,7 @@
         <v>101</v>
       </c>
       <c r="J14" s="62" t="s">
-        <v>114</v>
+        <v>253</v>
       </c>
       <c r="K14" s="55" t="s">
         <v>101</v>
@@ -2583,7 +2589,7 @@
         <v>82</v>
       </c>
       <c r="O14" s="74" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="P14" s="76" t="s">
         <v>101</v>
@@ -2592,19 +2598,19 @@
         <v>6</v>
       </c>
       <c r="R14" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S14" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T14" s="81" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="U14" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V14" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -2615,17 +2621,17 @@
         <v>102</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F15" s="74"/>
       <c r="G15" s="58" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H15" s="76">
         <v>13</v>
@@ -2634,7 +2640,7 @@
         <v>101</v>
       </c>
       <c r="J15" s="62" t="s">
-        <v>117</v>
+        <v>254</v>
       </c>
       <c r="K15" s="55" t="s">
         <v>101</v>
@@ -2647,7 +2653,7 @@
         <v>97</v>
       </c>
       <c r="O15" s="74" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="P15" s="76" t="s">
         <v>100</v>
@@ -2656,19 +2662,19 @@
         <v>6</v>
       </c>
       <c r="R15" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S15" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T15" s="81" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="U15" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V15" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -2679,17 +2685,17 @@
         <v>102</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F16" s="74"/>
       <c r="G16" s="58" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H16" s="76">
         <v>14</v>
@@ -2698,7 +2704,7 @@
         <v>101</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K16" s="55" t="s">
         <v>101</v>
@@ -2711,7 +2717,7 @@
         <v>94</v>
       </c>
       <c r="O16" s="74" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="P16" s="76" t="s">
         <v>101</v>
@@ -2720,19 +2726,19 @@
         <v>6</v>
       </c>
       <c r="R16" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S16" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T16" s="81" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="U16" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V16" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -2743,17 +2749,17 @@
         <v>102</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E17" s="63" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F17" s="74"/>
       <c r="G17" s="58" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="H17" s="76">
         <v>15</v>
@@ -2762,7 +2768,7 @@
         <v>101</v>
       </c>
       <c r="J17" s="62" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="K17" s="55" t="s">
         <v>101</v>
@@ -2775,7 +2781,7 @@
         <v>84</v>
       </c>
       <c r="O17" s="74" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="P17" s="76" t="s">
         <v>100</v>
@@ -2784,19 +2790,19 @@
         <v>6</v>
       </c>
       <c r="R17" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="S17" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="T17" s="81" t="s">
         <v>170</v>
       </c>
-      <c r="S17" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="T17" s="81" t="s">
-        <v>187</v>
-      </c>
       <c r="U17" s="79" t="s">
-        <v>179</v>
-      </c>
-      <c r="V17" s="103" t="s">
-        <v>268</v>
+        <v>162</v>
+      </c>
+      <c r="V17" s="89" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -2807,15 +2813,15 @@
         <v>102</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E18" s="63"/>
       <c r="F18" s="74"/>
       <c r="G18" s="58" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H18" s="76">
         <v>16</v>
@@ -2824,7 +2830,7 @@
         <v>100</v>
       </c>
       <c r="J18" s="62" t="s">
-        <v>124</v>
+        <v>255</v>
       </c>
       <c r="K18" s="55" t="s">
         <v>101</v>
@@ -2837,7 +2843,7 @@
       </c>
       <c r="N18" s="57"/>
       <c r="O18" s="74" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="P18" s="76" t="s">
         <v>100</v>
@@ -2846,19 +2852,19 @@
         <v>6</v>
       </c>
       <c r="R18" s="80" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="S18" s="79" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="T18" s="81" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="U18" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="V18" s="104" t="s">
-        <v>270</v>
+        <v>151</v>
+      </c>
+      <c r="V18" s="90" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -2869,17 +2875,17 @@
         <v>102</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E19" s="63" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F19" s="74"/>
       <c r="G19" s="58" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H19" s="76">
         <v>17</v>
@@ -2888,7 +2894,7 @@
         <v>101</v>
       </c>
       <c r="J19" s="62" t="s">
-        <v>126</v>
+        <v>256</v>
       </c>
       <c r="K19" s="55" t="s">
         <v>101</v>
@@ -2901,7 +2907,7 @@
         <v>97</v>
       </c>
       <c r="O19" s="74" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="P19" s="76" t="s">
         <v>100</v>
@@ -2910,19 +2916,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S19" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T19" s="81" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="U19" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V19" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -2933,19 +2939,19 @@
         <v>102</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D20" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="G20" s="58" t="s">
         <v>123</v>
-      </c>
-      <c r="F20" s="74" t="s">
-        <v>128</v>
-      </c>
-      <c r="G20" s="58" t="s">
-        <v>129</v>
       </c>
       <c r="H20" s="76">
         <v>18</v>
@@ -2954,7 +2960,7 @@
         <v>101</v>
       </c>
       <c r="J20" s="62" t="s">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c r="K20" s="55" t="s">
         <v>101</v>
@@ -2967,7 +2973,7 @@
         <v>82</v>
       </c>
       <c r="O20" s="74" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="P20" s="76" t="s">
         <v>101</v>
@@ -2976,19 +2982,19 @@
         <v>6</v>
       </c>
       <c r="R20" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S20" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T20" s="81" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="U20" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V20" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -2999,19 +3005,19 @@
         <v>102</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D21" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="E21" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" s="74" t="s">
-        <v>128</v>
-      </c>
       <c r="G21" s="58" t="s">
-        <v>130</v>
+        <v>273</v>
       </c>
       <c r="H21" s="76">
         <v>19</v>
@@ -3020,7 +3026,7 @@
         <v>101</v>
       </c>
       <c r="J21" s="62" t="s">
-        <v>131</v>
+        <v>258</v>
       </c>
       <c r="K21" s="55" t="s">
         <v>101</v>
@@ -3033,7 +3039,7 @@
         <v>95</v>
       </c>
       <c r="O21" s="74" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="P21" s="76" t="s">
         <v>101</v>
@@ -3042,19 +3048,19 @@
         <v>6</v>
       </c>
       <c r="R21" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S21" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T21" s="81" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="U21" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V21" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -3065,17 +3071,17 @@
         <v>102</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D22" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E22" s="63" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F22" s="74"/>
       <c r="G22" s="58" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="H22" s="76">
         <v>20</v>
@@ -3084,7 +3090,7 @@
         <v>101</v>
       </c>
       <c r="J22" s="62" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="K22" s="55" t="s">
         <v>101</v>
@@ -3097,7 +3103,7 @@
         <v>98</v>
       </c>
       <c r="O22" s="74" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="P22" s="76" t="s">
         <v>100</v>
@@ -3106,19 +3112,19 @@
         <v>6</v>
       </c>
       <c r="R22" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S22" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T22" s="81" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="U22" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V22" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -3129,17 +3135,17 @@
         <v>102</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D23" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E23" s="63" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F23" s="74"/>
       <c r="G23" s="58" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H23" s="76">
         <v>21</v>
@@ -3148,7 +3154,7 @@
         <v>101</v>
       </c>
       <c r="J23" s="62" t="s">
-        <v>140</v>
+        <v>259</v>
       </c>
       <c r="K23" s="55" t="s">
         <v>101</v>
@@ -3161,7 +3167,7 @@
         <v>82</v>
       </c>
       <c r="O23" s="74" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="P23" s="76" t="s">
         <v>100</v>
@@ -3170,19 +3176,19 @@
         <v>6</v>
       </c>
       <c r="R23" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S23" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T23" s="81" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="U23" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V23" s="59" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -3193,19 +3199,19 @@
         <v>102</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D24" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E24" s="63" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F24" s="74" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>138</v>
+        <v>274</v>
       </c>
       <c r="H24" s="76">
         <v>22</v>
@@ -3214,7 +3220,7 @@
         <v>100</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>141</v>
+        <v>260</v>
       </c>
       <c r="K24" s="55" t="s">
         <v>101</v>
@@ -3227,7 +3233,7 @@
       </c>
       <c r="N24" s="57"/>
       <c r="O24" s="74" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="P24" s="76" t="s">
         <v>100</v>
@@ -3236,19 +3242,19 @@
         <v>6</v>
       </c>
       <c r="R24" s="80" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="S24" s="79" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="T24" s="81" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="U24" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="V24" s="104" t="s">
-        <v>270</v>
+        <v>151</v>
+      </c>
+      <c r="V24" s="90" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -3259,19 +3265,19 @@
         <v>102</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D25" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E25" s="63" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F25" s="74" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G25" s="58" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H25" s="76">
         <v>23</v>
@@ -3280,7 +3286,7 @@
         <v>101</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>143</v>
+        <v>261</v>
       </c>
       <c r="K25" s="55" t="s">
         <v>101</v>
@@ -3293,7 +3299,7 @@
         <v>96</v>
       </c>
       <c r="O25" s="74" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="P25" s="76" t="s">
         <v>101</v>
@@ -3302,19 +3308,19 @@
         <v>6</v>
       </c>
       <c r="R25" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S25" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T25" s="81" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="U25" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V25" s="63" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3325,17 +3331,17 @@
         <v>102</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D26" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E26" s="63" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="F26" s="74"/>
       <c r="G26" s="58" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="H26" s="76">
         <v>24</v>
@@ -3344,7 +3350,7 @@
         <v>101</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="K26" s="55" t="s">
         <v>101</v>
@@ -3357,7 +3363,7 @@
         <v>82</v>
       </c>
       <c r="O26" s="74" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="P26" s="76" t="s">
         <v>100</v>
@@ -3366,19 +3372,19 @@
         <v>6</v>
       </c>
       <c r="R26" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S26" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T26" s="81" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="U26" s="79" t="s">
-        <v>179</v>
-      </c>
-      <c r="V26" s="104" t="s">
-        <v>270</v>
+        <v>162</v>
+      </c>
+      <c r="V26" s="90" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -3389,17 +3395,17 @@
         <v>102</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E27" s="63" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
       <c r="F27" s="74"/>
       <c r="G27" s="58" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="H27" s="76">
         <v>25</v>
@@ -3408,7 +3414,7 @@
         <v>101</v>
       </c>
       <c r="J27" s="62" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="K27" s="55" t="s">
         <v>101</v>
@@ -3421,7 +3427,7 @@
         <v>82</v>
       </c>
       <c r="O27" s="74" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="P27" s="76" t="s">
         <v>100</v>
@@ -3430,19 +3436,19 @@
         <v>6</v>
       </c>
       <c r="R27" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S27" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T27" s="81" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="U27" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V27" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -3456,14 +3462,14 @@
         <v>103</v>
       </c>
       <c r="D28" s="64" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="F28" s="74"/>
       <c r="G28" s="58" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="H28" s="76">
         <v>26</v>
@@ -3472,7 +3478,7 @@
         <v>100</v>
       </c>
       <c r="J28" s="62" t="s">
-        <v>154</v>
+        <v>263</v>
       </c>
       <c r="K28" s="55" t="s">
         <v>101</v>
@@ -3485,7 +3491,7 @@
       </c>
       <c r="N28" s="57"/>
       <c r="O28" s="74" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="P28" s="76" t="s">
         <v>100</v>
@@ -3494,19 +3500,19 @@
         <v>6</v>
       </c>
       <c r="R28" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S28" s="79" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="T28" s="81" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="U28" s="79" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="V28" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
@@ -3520,14 +3526,14 @@
         <v>103</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E29" s="63" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F29" s="74"/>
       <c r="G29" s="58" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="H29" s="76">
         <v>27</v>
@@ -3536,7 +3542,7 @@
         <v>101</v>
       </c>
       <c r="J29" s="62" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="K29" s="55" t="s">
         <v>101</v>
@@ -3549,7 +3555,7 @@
         <v>84</v>
       </c>
       <c r="O29" s="74" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="P29" s="76" t="s">
         <v>100</v>
@@ -3558,19 +3564,19 @@
         <v>6</v>
       </c>
       <c r="R29" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S29" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T29" s="81" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="U29" s="79" t="s">
-        <v>179</v>
-      </c>
-      <c r="V29" s="104" t="s">
-        <v>270</v>
+        <v>162</v>
+      </c>
+      <c r="V29" s="90" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
@@ -3584,14 +3590,14 @@
         <v>103</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E30" s="63" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F30" s="74"/>
       <c r="G30" s="58" t="s">
-        <v>150</v>
+        <v>264</v>
       </c>
       <c r="H30" s="76">
         <v>28</v>
@@ -3600,7 +3606,7 @@
         <v>101</v>
       </c>
       <c r="J30" s="62" t="s">
-        <v>151</v>
+        <v>265</v>
       </c>
       <c r="K30" s="55" t="s">
         <v>101</v>
@@ -3613,7 +3619,7 @@
         <v>84</v>
       </c>
       <c r="O30" s="74" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="P30" s="76" t="s">
         <v>101</v>
@@ -3622,19 +3628,19 @@
         <v>6</v>
       </c>
       <c r="R30" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S30" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T30" s="81" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="U30" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V30" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -3648,12 +3654,12 @@
         <v>103</v>
       </c>
       <c r="D31" s="64" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E31" s="63"/>
       <c r="F31" s="74"/>
       <c r="G31" s="58" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="H31" s="76">
         <v>29</v>
@@ -3662,7 +3668,7 @@
         <v>101</v>
       </c>
       <c r="J31" s="62" t="s">
-        <v>158</v>
+        <v>266</v>
       </c>
       <c r="K31" s="55" t="s">
         <v>101</v>
@@ -3675,7 +3681,7 @@
       </c>
       <c r="N31" s="57"/>
       <c r="O31" s="74" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="P31" s="76" t="s">
         <v>100</v>
@@ -3684,19 +3690,19 @@
         <v>6</v>
       </c>
       <c r="R31" s="80" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="S31" s="79" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="T31" s="81" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="U31" s="79" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="V31" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -3710,12 +3716,12 @@
         <v>103</v>
       </c>
       <c r="D32" s="64" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E32" s="63"/>
       <c r="F32" s="74"/>
       <c r="G32" s="58" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="H32" s="76">
         <v>30</v>
@@ -3724,7 +3730,7 @@
         <v>101</v>
       </c>
       <c r="J32" s="62" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="K32" s="55" t="s">
         <v>101</v>
@@ -3737,7 +3743,7 @@
         <v>86</v>
       </c>
       <c r="O32" s="74" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="P32" s="76" t="s">
         <v>100</v>
@@ -3746,19 +3752,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S32" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T32" s="81" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="U32" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V32" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -3772,12 +3778,12 @@
         <v>103</v>
       </c>
       <c r="D33" s="64" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E33" s="63"/>
       <c r="F33" s="74"/>
       <c r="G33" s="58" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="H33" s="76">
         <v>31</v>
@@ -3786,7 +3792,7 @@
         <v>101</v>
       </c>
       <c r="J33" s="62" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
       <c r="K33" s="55" t="s">
         <v>101</v>
@@ -3799,7 +3805,7 @@
         <v>86</v>
       </c>
       <c r="O33" s="74" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="P33" s="76" t="s">
         <v>100</v>
@@ -3808,19 +3814,19 @@
         <v>6</v>
       </c>
       <c r="R33" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S33" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T33" s="81" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="U33" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V33" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -3834,12 +3840,12 @@
         <v>103</v>
       </c>
       <c r="D34" s="64" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
       <c r="E34" s="63"/>
       <c r="F34" s="74"/>
       <c r="G34" s="58" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="H34" s="76">
         <v>32</v>
@@ -3848,7 +3854,7 @@
         <v>101</v>
       </c>
       <c r="J34" s="62" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="K34" s="55" t="s">
         <v>101</v>
@@ -3864,7 +3870,7 @@
       <c r="T34" s="81"/>
       <c r="U34" s="79"/>
       <c r="V34" s="59" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
@@ -3878,12 +3884,12 @@
         <v>103</v>
       </c>
       <c r="D35" s="64" t="s">
-        <v>257</v>
+        <v>230</v>
       </c>
       <c r="E35" s="63"/>
       <c r="F35" s="74"/>
       <c r="G35" s="58" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="H35" s="76">
         <v>33</v>
@@ -3892,7 +3898,7 @@
         <v>101</v>
       </c>
       <c r="J35" s="62" t="s">
-        <v>163</v>
+        <v>271</v>
       </c>
       <c r="K35" s="55" t="s">
         <v>101</v>
@@ -3912,19 +3918,19 @@
         <v>6</v>
       </c>
       <c r="R35" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S35" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T35" s="81" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="U35" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V35" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
@@ -3938,16 +3944,20 @@
         <v>103</v>
       </c>
       <c r="D36" s="64" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="E36" s="63"/>
       <c r="F36" s="74"/>
-      <c r="G36" s="58"/>
+      <c r="G36" s="58" t="s">
+        <v>269</v>
+      </c>
       <c r="H36" s="76">
         <v>34</v>
       </c>
       <c r="I36" s="76"/>
-      <c r="J36" s="62"/>
+      <c r="J36" s="62" t="s">
+        <v>272</v>
+      </c>
       <c r="K36" s="55"/>
       <c r="L36" s="56"/>
       <c r="M36" s="57"/>
@@ -3962,19 +3972,19 @@
         <v>6</v>
       </c>
       <c r="R36" s="80" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="S36" s="79" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="T36" s="81" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="U36" s="79" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="V36" s="59" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3984,7 +3994,7 @@
       <c r="D37" s="65"/>
       <c r="E37" s="66"/>
       <c r="F37" s="75"/>
-      <c r="G37" s="45"/>
+      <c r="G37" s="58"/>
       <c r="H37" s="77"/>
       <c r="I37" s="78"/>
       <c r="J37" s="67"/>
@@ -4139,34 +4149,34 @@
       <c r="U43" s="82"/>
     </row>
     <row r="44" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="89"/>
-      <c r="B44" s="89"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
-      <c r="G44" s="89"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="89"/>
-      <c r="J44" s="89"/>
-      <c r="K44" s="89"/>
+      <c r="A44" s="91"/>
+      <c r="B44" s="91"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="91"/>
+      <c r="E44" s="91"/>
+      <c r="F44" s="91"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="91"/>
+      <c r="K44" s="91"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="89"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="89"/>
-      <c r="G45" s="89"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
+      <c r="A45" s="91"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="91"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="91"/>
+      <c r="F45" s="91"/>
+      <c r="G45" s="91"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="91"/>
+      <c r="J45" s="91"/>
+      <c r="K45" s="91"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="P46" s="60" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>